<commit_message>
solve issue with computation safety stock
</commit_message>
<xml_diff>
--- a/Instances/SuperSmallIntance_Normal.xlsx
+++ b/Instances/SuperSmallIntance_Normal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCWam\DOCUME~1\MobaXterm\slash\RemoteFiles\329834_4_5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCWam\DOCUME~1\MobaXterm\slash\RemoteFiles\5508188_8_99\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="6360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -576,7 +576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>